<commit_message>
Fixed treatment subsetted physeq objects, fixed PERMANOVA pvals
</commit_message>
<xml_diff>
--- a/PERMANOVA.pvals.xlsx
+++ b/PERMANOVA.pvals.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{361F20A6-D1EE-4625-AAB6-80E0D9600591}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{044567BF-4D19-4D90-AD32-A73036FDB8F7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
-    <sheet name="PERMANOVA.pvals" sheetId="1" r:id="rId1"/>
+    <sheet name="PERMANOVA.pvals2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
   <si>
     <t>pvals</t>
   </si>
@@ -85,13 +85,7 @@
     <t>Stevia</t>
   </si>
   <si>
-    <t>Post Low Fat diff from everything</t>
-  </si>
-  <si>
-    <t>All treatments sig diff pre vs. post</t>
-  </si>
-  <si>
-    <t>Trend of diff btwn post saccharin vs. stevia</t>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -234,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,7 +410,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,9 +581,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -939,15 +940,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -961,12 +962,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1E-3</v>
       </c>
       <c r="B2" s="1">
-        <v>5.7142857142857099E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -974,17 +975,13 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1E-3</v>
       </c>
       <c r="B3" s="1">
-        <v>5.7142857142857099E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -992,17 +989,13 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>1E-3</v>
       </c>
       <c r="B4" s="1">
-        <v>5.7142857142857099E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1010,17 +1003,13 @@
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>1E-3</v>
       </c>
       <c r="B5" s="1">
-        <v>5.7142857142857099E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -1028,14 +1017,13 @@
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>1E-3</v>
       </c>
       <c r="B6" s="1">
-        <v>5.7142857142857099E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -1043,14 +1031,13 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>1E-3</v>
       </c>
       <c r="B7" s="1">
-        <v>5.7142857142857099E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -1058,14 +1045,13 @@
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>1E-3</v>
       </c>
       <c r="B8" s="1">
-        <v>5.7142857142857099E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -1073,89 +1059,83 @@
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.2500000000000003E-3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.8666666666666699E-2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.52E-2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>0.01</v>
       </c>
-      <c r="B9" s="1">
-        <v>3.6363636363636397E-2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0.01</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3.6363636363636397E-2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3.6363636363636397E-2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>8.9999999999999993E-3</v>
-      </c>
       <c r="B12" s="1">
-        <v>3.6363636363636397E-2</v>
+        <v>3.8181818181818199E-2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1.2E-2</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="B13" s="1">
-        <v>0.04</v>
+        <v>3.85E-2</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1.2999999999999999E-2</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>1.2E-2</v>
       </c>
       <c r="B14" s="1">
-        <v>0.04</v>
+        <v>3.8769230769230799E-2</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1163,87 +1143,86 @@
       <c r="D14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="B15">
-        <v>6.8571428571428603E-2</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" s="2">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="B16">
-        <v>7.7333333333333296E-2</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="B17">
-        <v>0.1275</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>5.5E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="B18">
-        <v>0.129411764705882</v>
+        <v>0.111176470588235</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>7.1999999999999995E-2</v>
+        <v>0.05</v>
       </c>
       <c r="B19">
-        <v>0.16</v>
+        <v>0.116666666666667</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0.11</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="B20">
-        <v>0.231578947368421</v>
+        <v>0.187894736842105</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1251,167 +1230,167 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>0.20499999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="B21">
-        <v>0.41</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0.221</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="B22">
-        <v>0.42095238095238102</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>0.24</v>
+        <v>0.184</v>
       </c>
       <c r="B23">
-        <v>0.43636363636363601</v>
+        <v>0.35127272727272701</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>0.26100000000000001</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="B24">
-        <v>0.453913043478261</v>
+        <v>0.3745</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>0.32800000000000001</v>
+        <v>0.214</v>
       </c>
       <c r="B25">
-        <v>0.54666666666666697</v>
+        <v>0.3745</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>0.38500000000000001</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="B26">
-        <v>0.59230769230769198</v>
+        <v>0.43008000000000002</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>0.374</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="B27">
-        <v>0.59230769230769198</v>
+        <v>0.54438461538461502</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>0.40500000000000003</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="B28">
-        <v>0.6</v>
+        <v>0.57062068965517199</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>0.443</v>
+        <v>0.37</v>
       </c>
       <c r="B29">
-        <v>0.63285714285714301</v>
+        <v>0.57062068965517199</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0.47499999999999998</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="B30">
-        <v>0.65517241379310298</v>
+        <v>0.57062068965517199</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0.50600000000000001</v>
+        <v>0.437</v>
       </c>
       <c r="B31">
-        <v>0.67466666666666697</v>
+        <v>0.61180000000000001</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>0.63400000000000001</v>
+        <v>0.505</v>
       </c>
       <c r="B32">
-        <v>0.81806451612903197</v>
+        <v>0.68419354838709701</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
@@ -1419,13 +1398,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>0.66</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="B33">
-        <v>0.821818181818182</v>
+        <v>0.71006250000000004</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -1433,27 +1412,27 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>0.67800000000000005</v>
+        <v>0.65</v>
       </c>
       <c r="B34">
-        <v>0.821818181818182</v>
+        <v>0.80294117647058805</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>0.84099999999999997</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="B35">
-        <v>0.88717948717948703</v>
+        <v>0.80294117647058805</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -1461,69 +1440,69 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>0.86499999999999999</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="B36">
-        <v>0.88717948717948703</v>
+        <v>0.83760000000000001</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>0.77500000000000002</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="B37">
-        <v>0.88717948717948703</v>
+        <v>0.89016666666666699</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>0.81200000000000006</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="B38">
-        <v>0.88717948717948703</v>
+        <v>0.89335135135135102</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>0.84299999999999997</v>
+        <v>0.877</v>
       </c>
       <c r="B39">
-        <v>0.88717948717948703</v>
+        <v>0.89839024390243905</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>0.82499999999999996</v>
+        <v>0.874</v>
       </c>
       <c r="B40">
-        <v>0.88717948717948703</v>
+        <v>0.89839024390243905</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1531,20 +1510,48 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>0.95199999999999996</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="B41">
-        <v>0.95199999999999996</v>
+        <v>0.89839024390243905</v>
       </c>
       <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0.83</v>
+      </c>
+      <c r="B42">
+        <v>0.89839024390243905</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="B43">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D41">
+  <sortState ref="A2:D43">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>